<commit_message>
fix: change fixtures files test
</commit_message>
<xml_diff>
--- a/cypress/fixtures/wrong_heads_template.xlsx
+++ b/cypress/fixtures/wrong_heads_template.xlsx
@@ -7,73 +7,48 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="S2DX5x4SmOQAQxtVA5XNknc+YPEX8Aazi5QwbdUk2Hc="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ref</t>
   </si>
   <si>
-    <t>firstName</t>
+    <t>first_name__</t>
   </si>
   <si>
-    <t>last_name</t>
+    <t>last_namess</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>entranceDatetime</t>
+    <t>entrance_datetime</t>
   </si>
   <si>
-    <t>STD000001</t>
+    <t>sex</t>
   </si>
   <si>
-    <t>John</t>
+    <t>test-</t>
   </si>
   <si>
-    <t>Smith</t>
+    <t>c1c1c1c</t>
   </si>
   <si>
-    <t>2023-02-28</t>
+    <t>lol</t>
   </si>
   <si>
-    <t>STD000002</t>
+    <t>c2@gmail.com</t>
   </si>
   <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t>STD000003</t>
-  </si>
-  <si>
-    <t>Jeanne</t>
-  </si>
-  <si>
-    <t>STD000004</t>
-  </si>
-  <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>STD000005</t>
-  </si>
-  <si>
-    <t>Pierre</t>
-  </si>
-  <si>
-    <t>STD000006</t>
-  </si>
-  <si>
-    <t>Hélène</t>
-  </si>
-  <si>
-    <t>STD000007</t>
-  </si>
-  <si>
-    <t>Patrice</t>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -81,9 +56,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd-mm-yy"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -94,11 +69,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,16 +85,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -342,7 +309,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="26.0"/>
+    <col customWidth="1" min="5" max="5" width="19.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -352,246 +319,38 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f t="shared" ref="D2:D13" si="1">CONCATENATE("user",A2,"@hei.school")</f>
-        <v>userSTD000001@hei.school</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E2" s="3">
+        <v>44927.0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000002@hei.school</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000003@hei.school</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000004@hei.school</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000005@hei.school</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000006@hei.school</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000007@hei.school</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000003@hei.school</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000004@hei.school</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000005@hei.school</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000006@hei.school</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000007@hei.school</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16">
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17">
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18">
-      <c r="E18" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
feat: import button xlsx
* feat: creat import button

* fix: fix import button

* style: refactor the code with prettier

* fix: change fixtures files test
</commit_message>
<xml_diff>
--- a/cypress/fixtures/wrong_heads_template.xlsx
+++ b/cypress/fixtures/wrong_heads_template.xlsx
@@ -7,73 +7,48 @@
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="S2DX5x4SmOQAQxtVA5XNknc+YPEX8Aazi5QwbdUk2Hc="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ref</t>
   </si>
   <si>
-    <t>firstName</t>
+    <t>first_name__</t>
   </si>
   <si>
-    <t>last_name</t>
+    <t>last_namess</t>
   </si>
   <si>
     <t>email</t>
   </si>
   <si>
-    <t>entranceDatetime</t>
+    <t>entrance_datetime</t>
   </si>
   <si>
-    <t>STD000001</t>
+    <t>sex</t>
   </si>
   <si>
-    <t>John</t>
+    <t>test-</t>
   </si>
   <si>
-    <t>Smith</t>
+    <t>c1c1c1c</t>
   </si>
   <si>
-    <t>2023-02-28</t>
+    <t>lol</t>
   </si>
   <si>
-    <t>STD000002</t>
+    <t>c2@gmail.com</t>
   </si>
   <si>
-    <t>Patrick</t>
-  </si>
-  <si>
-    <t>STD000003</t>
-  </si>
-  <si>
-    <t>Jeanne</t>
-  </si>
-  <si>
-    <t>STD000004</t>
-  </si>
-  <si>
-    <t>Jean</t>
-  </si>
-  <si>
-    <t>STD000005</t>
-  </si>
-  <si>
-    <t>Pierre</t>
-  </si>
-  <si>
-    <t>STD000006</t>
-  </si>
-  <si>
-    <t>Hélène</t>
-  </si>
-  <si>
-    <t>STD000007</t>
-  </si>
-  <si>
-    <t>Patrice</t>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -81,9 +56,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd-mm-yy"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="12.0"/>
       <color theme="1"/>
@@ -94,11 +69,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,16 +85,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -342,7 +309,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="26.0"/>
+    <col customWidth="1" min="5" max="5" width="19.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -352,246 +319,38 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f t="shared" ref="D2:D13" si="1">CONCATENATE("user",A2,"@hei.school")</f>
-        <v>userSTD000001@hei.school</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="E2" s="3">
+        <v>44927.0</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000002@hei.school</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000003@hei.school</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000004@hei.school</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000005@hei.school</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000006@hei.school</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000007@hei.school</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000003@hei.school</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000004@hei.school</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000005@hei.school</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000006@hei.school</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>userSTD000007@hei.school</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16">
-      <c r="E16" s="4"/>
-    </row>
-    <row r="17">
-      <c r="E17" s="4"/>
-    </row>
-    <row r="18">
-      <c r="E18" s="4"/>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>

</xml_diff>